<commit_message>
new test and training .ex files
</commit_message>
<xml_diff>
--- a/CMCM Lab Associative Learning Study Counterbalacing.xlsx
+++ b/CMCM Lab Associative Learning Study Counterbalacing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoanneMiao/Desktop/CMCM JM Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoanneMiao/Desktop/CMCM JM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6486B89-52C3-5E4E-B40A-032B868BA20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEC0D20-CB87-2D49-956D-734B66848326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{417284C1-A0D2-4539-9F2E-FC16F8FBD9EA}"/>
   </bookViews>
@@ -6324,7 +6324,7 @@
   <dimension ref="A1:AT56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>